<commit_message>
Additional Updates to Installation Procedure, Water Block Sight Glass Camera, and Addition of Navy Reports to Calibration Report Utility
</commit_message>
<xml_diff>
--- a/Addition of Navy Reports to Calibration Report Utility/Supporting Documentation/Example/2024-07-08/570 Ton Production_2024_07_08.xlsx
+++ b/Addition of Navy Reports to Calibration Report Utility/Supporting Documentation/Example/2024-07-08/570 Ton Production_2024_07_08.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://mysite.jci.com/personal/jbeachsc_jci_com/Documents/Documents/Projects/Addition of Navy Reports to Calibration Report Utility/Supporting Documentation/Example/2024-07-08/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="21" documentId="8_{15150D3B-1482-4E5A-B311-29E2D5C54519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B1B3D604-D778-4848-9931-24629AE3F370}"/>
+  <xr:revisionPtr revIDLastSave="27" documentId="8_{15150D3B-1482-4E5A-B311-29E2D5C54519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8C347FEC-EC79-4945-819D-D09726BFD3E9}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="4845" windowWidth="29040" windowHeight="15840" tabRatio="678" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="4845" windowWidth="29040" windowHeight="15840" tabRatio="678" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Report Template" sheetId="1" r:id="rId1"/>
@@ -4219,6 +4219,10 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
@@ -4521,8 +4525,8 @@
   </sheetPr>
   <dimension ref="A1:G70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D57" sqref="D57"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5600,8 +5604,8 @@
   </sheetPr>
   <dimension ref="A1:O87"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="C70" sqref="C70"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -11266,15 +11270,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:Y134"/>
   <sheetViews>
-    <sheetView topLeftCell="A82" workbookViewId="0">
-      <selection sqref="A1:Y134"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="4" max="4" width="36.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="34.42578125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="37.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="26" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="6.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
@@ -19916,30 +19941,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="f2a00314-ae30-474d-911b-f8e025e1af2d" ContentTypeId="0x010100EA254AAEB50D427F87E6DD3EC4BD2437" PreviousValue="false"/>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<customXsn xmlns="http://schemas.microsoft.com/office/2006/metadata/customXsn">
-  <xsnLocation/>
-  <cached>True</cached>
-  <openByDefault>True</openByDefault>
-  <xsnScope/>
-</customXsn>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="JCI Document" ma:contentTypeID="0x010100EA254AAEB50D427F87E6DD3EC4BD243700E9DE5F98739F3B429380BCA2E3696BC2" ma:contentTypeVersion="5" ma:contentTypeDescription="JCI Document" ma:contentTypeScope="" ma:versionID="3955ada78c24239fa9700bbfd7f7934b">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="9c4207fe-393b-4012-82d4-488376c51aab" xmlns:ns3="e3e2664a-4298-401e-9fa6-8f5325dd2938" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="50021d37a7b8ab4183afcb8aff0b29f5" ns2:_="" ns3:_="">
     <xsd:import namespace="9c4207fe-393b-4012-82d4-488376c51aab"/>
@@ -20116,7 +20117,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <JCILocationTaxHTField0 xmlns="9c4207fe-393b-4012-82d4-488376c51aab">
@@ -20139,31 +20140,31 @@
 </p:properties>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3109AC88-0E60-488C-8AC3-018832548145}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70270C07-0F4E-475D-ABEF-EBCA88CCD3E8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<SharedContentType xmlns="Microsoft.SharePoint.Taxonomy.ContentTypeSync" SourceId="f2a00314-ae30-474d-911b-f8e025e1af2d" ContentTypeId="0x010100EA254AAEB50D427F87E6DD3EC4BD2437" PreviousValue="false"/>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75DFDF45-1E46-469B-B7AF-371ED483F09D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/customXsn"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item5.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<customXsn xmlns="http://schemas.microsoft.com/office/2006/metadata/customXsn">
+  <xsnLocation/>
+  <cached>True</cached>
+  <openByDefault>True</openByDefault>
+  <xsnScope/>
+</customXsn>
 </file>
 
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95CE8855-DAB9-4D18-B52A-3F140E85C364}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -20182,7 +20183,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7BB540BB-0801-4752-8CD2-070B7A123846}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
@@ -20197,4 +20198,28 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3109AC88-0E60-488C-8AC3-018832548145}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70270C07-0F4E-475D-ABEF-EBCA88CCD3E8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="Microsoft.SharePoint.Taxonomy.ContentTypeSync"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps5.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{75DFDF45-1E46-469B-B7AF-371ED483F09D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/customXsn"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>